<commit_message>
Deploying to gh-pages from  @ 2bc519b448febf266acedfb34d300b23bc1e15a8 🚀
</commit_message>
<xml_diff>
--- a/notebooks/Exercises/exercise_02_Sol.xlsx
+++ b/notebooks/Exercises/exercise_02_Sol.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Work\Teaching\FINC462_662\Github_Coursepage\notebooks\Exercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE74B40-A348-451C-9B94-836C65DD25C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C506F4B1-82F1-4154-BE14-EC79D3830A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="885" windowWidth="20100" windowHeight="18600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9825" yWindow="720" windowWidth="28020" windowHeight="16485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Solutions" sheetId="1" r:id="rId1"/>
@@ -338,9 +338,6 @@
     <t>The annuity starts 21 years from now and ends after 24 payments (i.e. it ends in year 45)</t>
   </si>
   <si>
-    <t>The PV of this annuity at the start of year 20 is</t>
-  </si>
-  <si>
     <t>=137986.42/(1.05)^21</t>
   </si>
   <si>
@@ -393,6 +390,9 @@
   </si>
   <si>
     <t>FINC 462/662: Exercise 02 Detailed Solutions</t>
+  </si>
+  <si>
+    <t>The PV of this annuity at the start of year 21 is</t>
   </si>
 </sst>
 </file>
@@ -402,7 +402,7 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -499,7 +499,7 @@
     <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -1869,8 +1869,8 @@
   </sheetPr>
   <dimension ref="A1:G206"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A166" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B186" sqref="B186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1890,7 +1890,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -1907,15 +1907,15 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1926,10 +1926,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1940,15 +1940,15 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1964,10 +1964,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1978,15 +1978,15 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D22" s="2">
         <f xml:space="preserve"> 20/0.05 * (1 - 1/(1+0.05)^10)</f>
@@ -1995,7 +1995,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D23" s="2">
         <f>1/(1+0.05)^(10) * (4.17/0.05*(1-1/(1+0.05)^24))</f>
@@ -2004,7 +2004,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D24" s="2">
         <f>1/(1+0.05)^10*(20/0.05*(1-1/(1+0.05)^3))</f>
@@ -2013,7 +2013,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D25" s="4">
         <f>SUM(D22:D24)</f>
@@ -2790,7 +2790,7 @@
       <c r="F169" s="2"/>
       <c r="G169" s="2"/>
     </row>
-    <row r="170" spans="1:7" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2"/>
       <c r="B170" s="6">
         <f>B166/(1+0.05)^5</f>
@@ -2856,33 +2856,33 @@
       <c r="F175" s="2"/>
       <c r="G175" s="2"/>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="1"/>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="1"/>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B184" s="6">
         <f>10000/0.05*(1 - 1/(1.05)^24)</f>
         <v>137986.41794346995</v>
@@ -2891,23 +2891,27 @@
         <v>79</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B186" s="6">
         <f>B184/(1.05)^21</f>
         <v>49529.171144963926</v>
       </c>
       <c r="C186" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="D186" s="2">
+        <f>10000/0.05*(1 - 1/(1.05)^45)-10000/0.05*(1 - 1/(1.05)^21)</f>
+        <v>49529.171144963926</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="200" spans="3:5" x14ac:dyDescent="0.25">

</xml_diff>